<commit_message>
better excel formatting and styling
</commit_message>
<xml_diff>
--- a/dist/output.xlsx
+++ b/dist/output.xlsx
@@ -415,7 +415,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -423,9 +423,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="12.65" customWidth="1" min="3" max="3"/>
-    <col width="6.899999999999999" customWidth="1" min="4" max="4"/>
-    <col width="9.199999999999999" customWidth="1" min="5" max="5"/>
+    <col width="8.049999999999999" customWidth="1" min="3" max="3"/>
   </cols>
   <sheetData>
     <row r="1"/>
@@ -435,7 +433,7 @@
     <row r="5">
       <c r="C5" s="1" t="inlineStr">
         <is>
-          <t>Monday</t>
+          <t>Tuesday</t>
         </is>
       </c>
     </row>
@@ -443,25 +441,7 @@
     <row r="7">
       <c r="C7" s="1" t="inlineStr">
         <is>
-          <t>Chest</t>
-        </is>
-      </c>
-    </row>
-    <row r="8"/>
-    <row r="9">
-      <c r="C9" s="1" t="inlineStr">
-        <is>
-          <t>Bench Press</t>
-        </is>
-      </c>
-      <c r="D9" s="1" t="inlineStr">
-        <is>
-          <t>3 sets</t>
-        </is>
-      </c>
-      <c r="E9" s="1" t="inlineStr">
-        <is>
-          <t>4-6 reps</t>
+          <t>asdsads</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
better gui handling of workouts
</commit_message>
<xml_diff>
--- a/dist/output.xlsx
+++ b/dist/output.xlsx
@@ -415,7 +415,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -423,7 +423,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="8.049999999999999" customWidth="1" min="3" max="3"/>
+    <col width="14.95" customWidth="1" min="3" max="3"/>
+    <col width="6.899999999999999" customWidth="1" min="4" max="4"/>
+    <col width="9.199999999999999" customWidth="1" min="5" max="5"/>
   </cols>
   <sheetData>
     <row r="1"/>
@@ -433,7 +435,7 @@
     <row r="5">
       <c r="C5" s="1" t="inlineStr">
         <is>
-          <t>Tuesday</t>
+          <t>Monday</t>
         </is>
       </c>
     </row>
@@ -441,7 +443,42 @@
     <row r="7">
       <c r="C7" s="1" t="inlineStr">
         <is>
-          <t>asdsads</t>
+          <t>Chest</t>
+        </is>
+      </c>
+    </row>
+    <row r="8"/>
+    <row r="9">
+      <c r="C9" s="1" t="inlineStr">
+        <is>
+          <t>Bench</t>
+        </is>
+      </c>
+      <c r="D9" s="1" t="inlineStr">
+        <is>
+          <t>3 sets</t>
+        </is>
+      </c>
+      <c r="E9" s="1" t="inlineStr">
+        <is>
+          <t>5-6 reps</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="C10" s="1" t="inlineStr">
+        <is>
+          <t>Incline Bench</t>
+        </is>
+      </c>
+      <c r="D10" s="1" t="inlineStr">
+        <is>
+          <t>3 sets</t>
+        </is>
+      </c>
+      <c r="E10" s="1" t="inlineStr">
+        <is>
+          <t>5-6 reps</t>
         </is>
       </c>
     </row>

</xml_diff>